<commit_message>
UAT, report, demo video pdf
</commit_message>
<xml_diff>
--- a/Project Development Phase/User Acceptance Testing/Testcases Report.xlsx
+++ b/Project Development Phase/User Acceptance Testing/Testcases Report.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958044AA-83BC-4198-9965-A5D413E6744D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A887456D-E319-4AB7-85D2-8A31039E6192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Shopenzer Testcases" sheetId="1" r:id="rId1"/>
-    <sheet name="Testscearnios" sheetId="3" r:id="rId2"/>
+    <sheet name="Car Resale Predictor Testcases" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Scenarios" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -2145,7 +2145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
@@ -2657,8 +2657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:B12"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>